<commit_message>
modified electricity price: flat price
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_EnergyPrice.xlsx
+++ b/data/input_operation/OperationScenario_Component_EnergyPrice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/Flex/data/input_operation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D75B27-C68B-7340-801C-301B7A14C30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EEBB34-9D46-0043-90D1-CA90CBD40CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="19200" windowHeight="6360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -881,7 +881,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -912,7 +912,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>1</v>

</xml_diff>